<commit_message>
Working on datasheet based calculations
</commit_message>
<xml_diff>
--- a/12V_Module/DatasheetDesign.xlsx
+++ b/12V_Module/DatasheetDesign.xlsx
@@ -1,26 +1,215 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\SW8E-MainPowerBoard\12V_Module\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5129B0-F190-42EF-A29F-46AA7FA01B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LM5156H_Datasheet_Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+  <si>
+    <t>Vin (min)</t>
+  </si>
+  <si>
+    <t>Vin (max)</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>Iout (max)</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>R_UVLOT</t>
+  </si>
+  <si>
+    <t>R_UVLOB</t>
+  </si>
+  <si>
+    <t>Ohms</t>
+  </si>
+  <si>
+    <t>Device Properties (Constants)</t>
+  </si>
+  <si>
+    <t>V_UVLO (falling)</t>
+  </si>
+  <si>
+    <t>V_UVLO (rising)</t>
+  </si>
+  <si>
+    <t>I_UVLO</t>
+  </si>
+  <si>
+    <t>UVLO Design</t>
+  </si>
+  <si>
+    <t>V_SUPPLY (ON)</t>
+  </si>
+  <si>
+    <t>V_SUPPLY (OFF)</t>
+  </si>
+  <si>
+    <t>C_UVLO</t>
+  </si>
+  <si>
+    <t>R_UVLOS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>These voltages selected as they avoiddamage by overcurrenting FET, inductor, diode, etc</t>
+  </si>
+  <si>
+    <t>Datasheet states these may be needed, but don't provide may specifics for when…</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>BIAS, VCC Design</t>
+  </si>
+  <si>
+    <t>C_VCC</t>
+  </si>
+  <si>
+    <t>Datasheet recommends 1uF to 4.7uF</t>
+  </si>
+  <si>
+    <t>SS Pin</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Design Parameters</t>
+  </si>
+  <si>
+    <t>I_SS</t>
+  </si>
+  <si>
+    <t>C_SS</t>
+  </si>
+  <si>
+    <t>Desired Soft Start Time (t_SS)</t>
+  </si>
+  <si>
+    <t>RT Pin</t>
+  </si>
+  <si>
+    <t>R_T</t>
+  </si>
+  <si>
+    <t>f_SW</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>f_RT</t>
+  </si>
+  <si>
+    <t>Same as f_RT b/c clock sync not used</t>
+  </si>
+  <si>
+    <t>DRSS</t>
+  </si>
+  <si>
+    <t>Connect DITHOFF to VCC</t>
+  </si>
+  <si>
+    <t>This disables DRSS</t>
+  </si>
+  <si>
+    <t>Clock Synchronization</t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>Not used. UVLO / SYNC connected with components previously calculated</t>
+  </si>
+  <si>
+    <t>CS Pin</t>
+  </si>
+  <si>
+    <t>Same as f_SW b/c clock sync not used</t>
+  </si>
+  <si>
+    <t>V_D1</t>
+  </si>
+  <si>
+    <t>Voltage drop across output  diode D1</t>
+  </si>
+  <si>
+    <t>I_SLOPE</t>
+  </si>
+  <si>
+    <t>V_SLOPE</t>
+  </si>
+  <si>
+    <t>f_SYNC</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>R_S (max)</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Selected RS</t>
+  </si>
+  <si>
+    <t>TODO SOME OF THIS IS INCORRECT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +217,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -45,12 +248,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +372,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>280496</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>45981</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325F69BB-9193-F8FA-D10C-45A46D28A154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6728460" y="1836420"/>
+          <a:ext cx="3305636" cy="1867161"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>124433</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>4142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{608F6E93-32C6-9988-97ED-6104E60DBEBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6743700" y="0"/>
+          <a:ext cx="4353533" cy="2381582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>143576</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>128011</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA6CF2A-B2F1-13EE-01E4-6C661F2ADDC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="10241280"/>
+          <a:ext cx="5020376" cy="2695951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +773,505 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1.575</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1.37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3">
+        <f>B13</f>
+        <v>1000000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3.3000000000000002E-6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3">
+        <f>(B21*(B2/B3)-B22)/B4</f>
+        <v>409489.05109489034</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3">
+        <f>(B3*B23)/(B21-B3)</f>
+        <v>99644.760213143833</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2.2000000000000001E-6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="3">
+        <f>(B12/1000)*B5</f>
+        <v>2.0000000000000002E-7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3">
+        <f>(22100000000/B14)-955</f>
+        <v>21145</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="3">
+        <f>B14</f>
+        <v>1000000</v>
+      </c>
+      <c r="C52" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="19"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="13">
+        <f>(0.00003)*(B14/B52)</f>
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="13">
+        <f>(0.04)*(B14/B52)</f>
+        <v>0.04</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="11"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="13">
+        <f>((0.08)*B13*B16)/(B59*((B10+B15)-B8))</f>
+        <v>4.7826086956521748E-2</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D53:H54"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="D21:H22"/>
+    <mergeCell ref="D25:H26"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D47:H47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>